<commit_message>
Updated to eps-1.4.3-california-wipF as provided by Chris on 11/14/20
</commit_message>
<xml_diff>
--- a/InputData/bldgs/ECiCpCU/Embedded Carbon in Components per Currency Unit.xlsx
+++ b/InputData/bldgs/ECiCpCU/Embedded Carbon in Components per Currency Unit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="21075" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="19440" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Source:</t>
-  </si>
-  <si>
     <t>Note:</t>
   </si>
   <si>
@@ -50,10 +47,13 @@
     <t>Embedded tons CO2/2012$</t>
   </si>
   <si>
-    <t>Most building components will be produced outside of the boundaries of the model.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It would not be appropriate to apply the California carbon tax to these emissions. </t>
+    <t>It is assumed that most of these emissions will be outside of California's boundaries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under these assumptions, it would not be appropriate to apply the California carbon price to these embedded emissions. </t>
+  </si>
+  <si>
+    <t>They are approximated as zero.</t>
   </si>
 </sst>
 </file>
@@ -63,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,14 +75,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,32 +156,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -197,15 +184,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
+    <cellStyle name="Footnotes: top row" xfId="6"/>
+    <cellStyle name="Header: bottom row" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="5"/>
+    <cellStyle name="Table title" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,47 +501,41 @@
     <col min="2" max="2" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-    </row>
-    <row r="19" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-    </row>
-    <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+    <row r="10" spans="1:1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -567,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -578,58 +558,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="6">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>